<commit_message>
Player Data Updated till 19 March 2023
</commit_message>
<xml_diff>
--- a/AFG_Player_Data.xlsx
+++ b/AFG_Player_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Misc\Machine_Deep_Learning\Cricket_Scout\Team_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Misc\Machine_Deep_Learning\Cricket_Scout\main\MatchConRep\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="PlayerCountryList.asp?Country_AFG_Comp_O_Current_T" localSheetId="0">Sheet1!$A$1:$P$27</definedName>
+    <definedName name="PlayerCountryList.asp?Country_AFG_Comp_O_Current_T" localSheetId="0">Sheet1!$A$1:$P$30</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="154">
   <si>
     <t>Name</t>
   </si>
@@ -458,7 +458,49 @@
     <t>0/22</t>
   </si>
   <si>
-    <t>Total Players = 25</t>
+    <t>A M Ghazanfar*</t>
+  </si>
+  <si>
+    <t>A M Ghazanfar</t>
+  </si>
+  <si>
+    <t>15/07/2007</t>
+  </si>
+  <si>
+    <t>2024-</t>
+  </si>
+  <si>
+    <t>0/13</t>
+  </si>
+  <si>
+    <t>5/17</t>
+  </si>
+  <si>
+    <t>Nangeyalia Kharote*</t>
+  </si>
+  <si>
+    <t>Nangeyalia Kharote</t>
+  </si>
+  <si>
+    <t>25/04/2004</t>
+  </si>
+  <si>
+    <t>10*</t>
+  </si>
+  <si>
+    <t>Naveed Zadran*</t>
+  </si>
+  <si>
+    <t>Naveed Zadran</t>
+  </si>
+  <si>
+    <t>07/03/2005</t>
+  </si>
+  <si>
+    <t>0/21</t>
+  </si>
+  <si>
+    <t>Total Players = 28</t>
   </si>
 </sst>
 </file>
@@ -780,9 +822,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -910,13 +952,13 @@
         <v>23</v>
       </c>
       <c r="E3">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F3">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G3">
-        <v>696</v>
+        <v>719</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -925,19 +967,19 @@
         <v>149</v>
       </c>
       <c r="J3">
-        <v>53.54</v>
+        <v>47.93</v>
       </c>
       <c r="K3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>47.75</v>
+        <v>45.78</v>
       </c>
       <c r="N3">
-        <v>5.89</v>
+        <v>5.7</v>
       </c>
       <c r="O3" t="s">
         <v>24</v>
@@ -1004,13 +1046,13 @@
         <v>33</v>
       </c>
       <c r="E5">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F5">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G5">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1019,19 +1061,19 @@
         <v>6</v>
       </c>
       <c r="J5">
-        <v>3.2</v>
+        <v>4.2</v>
       </c>
       <c r="K5">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="L5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M5">
-        <v>32</v>
+        <v>30.05</v>
       </c>
       <c r="N5">
-        <v>5.62</v>
+        <v>5.58</v>
       </c>
       <c r="O5" t="s">
         <v>34</v>
@@ -1039,128 +1081,128 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>140</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>141</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>142</v>
       </c>
       <c r="E6">
-        <v>81</v>
+        <v>2</v>
       </c>
       <c r="F6">
-        <v>70</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>1223</v>
+        <v>5</v>
       </c>
       <c r="H6">
         <v>0</v>
       </c>
-      <c r="I6">
-        <v>82</v>
+      <c r="I6" t="s">
+        <v>133</v>
       </c>
       <c r="J6">
-        <v>19.73</v>
+        <v>5</v>
       </c>
       <c r="K6">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="L6">
-        <v>4</v>
-      </c>
-      <c r="M6">
-        <v>35.57</v>
+        <v>0</v>
+      </c>
+      <c r="M6" t="s">
+        <v>44</v>
       </c>
       <c r="N6">
-        <v>5.54</v>
+        <v>5.22</v>
       </c>
       <c r="O6" t="s">
-        <v>39</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E7">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="F7">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="G7">
-        <v>2106</v>
+        <v>1231</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="J7">
-        <v>32.909999999999997</v>
+        <v>19.850000000000001</v>
       </c>
       <c r="K7">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7" t="s">
-        <v>44</v>
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>35.6</v>
       </c>
       <c r="N7">
-        <v>8.33</v>
+        <v>5.55</v>
       </c>
       <c r="O7" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D8" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E8">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="F8">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="G8">
-        <v>1358</v>
+        <v>2225</v>
       </c>
       <c r="H8">
-        <v>5</v>
-      </c>
-      <c r="I8" t="s">
-        <v>50</v>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>97</v>
       </c>
       <c r="J8">
-        <v>48.5</v>
+        <v>34.229999999999997</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1171,40 +1213,43 @@
       <c r="M8" t="s">
         <v>44</v>
       </c>
-      <c r="N8" t="s">
-        <v>44</v>
+      <c r="N8">
+        <v>8.33</v>
+      </c>
+      <c r="O8" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
         <v>49</v>
       </c>
       <c r="E9">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="F9">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="G9">
-        <v>373</v>
+        <v>1440</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="J9">
-        <v>26.64</v>
+        <v>48</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -1221,34 +1266,34 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="G10">
-        <v>32</v>
+        <v>375</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="J10">
-        <v>10.67</v>
+        <v>25</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1259,510 +1304,510 @@
       <c r="M10" t="s">
         <v>44</v>
       </c>
-      <c r="N10">
-        <v>6.92</v>
-      </c>
-      <c r="O10" t="s">
-        <v>60</v>
+      <c r="N10" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="E11">
-        <v>159</v>
+        <v>3</v>
       </c>
       <c r="F11">
-        <v>140</v>
+        <v>3</v>
       </c>
       <c r="G11">
-        <v>3359</v>
+        <v>32</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J11">
-        <v>26.87</v>
+        <v>10.67</v>
       </c>
       <c r="K11">
-        <v>164</v>
+        <v>0</v>
       </c>
       <c r="L11">
-        <v>4</v>
-      </c>
-      <c r="M11">
-        <v>32.659999999999997</v>
+        <v>0</v>
+      </c>
+      <c r="M11" t="s">
+        <v>44</v>
       </c>
       <c r="N11">
-        <v>4.29</v>
+        <v>6.92</v>
       </c>
       <c r="O11" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="E12">
+        <v>161</v>
+      </c>
+      <c r="F12">
+        <v>142</v>
+      </c>
+      <c r="G12">
+        <v>3447</v>
+      </c>
+      <c r="H12">
         <v>2</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
       <c r="I12" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="J12">
-        <v>0</v>
+        <v>27.14</v>
       </c>
       <c r="K12">
-        <v>0</v>
+        <v>169</v>
       </c>
       <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12" t="s">
-        <v>44</v>
+        <v>5</v>
+      </c>
+      <c r="M12">
+        <v>32.01</v>
       </c>
       <c r="N12">
-        <v>6.77</v>
+        <v>4.2699999999999996</v>
       </c>
       <c r="O12" t="s">
-        <v>71</v>
+        <v>144</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D13" t="s">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="E13">
-        <v>75</v>
+        <v>2</v>
       </c>
       <c r="F13">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="G13">
-        <v>236</v>
+        <v>0</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="J13">
-        <v>9.08</v>
+        <v>0</v>
       </c>
       <c r="K13">
-        <v>101</v>
+        <v>0</v>
       </c>
       <c r="L13">
-        <v>4</v>
-      </c>
-      <c r="M13">
-        <v>28.35</v>
+        <v>0</v>
+      </c>
+      <c r="M13" t="s">
+        <v>44</v>
       </c>
       <c r="N13">
-        <v>4.33</v>
+        <v>6.77</v>
       </c>
       <c r="O13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="E14">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="F14">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="G14">
-        <v>2060</v>
+        <v>236</v>
       </c>
       <c r="H14">
-        <v>1</v>
-      </c>
-      <c r="I14">
-        <v>104</v>
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>75</v>
       </c>
       <c r="J14">
-        <v>29.01</v>
+        <v>9.08</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>101</v>
       </c>
       <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="M14" t="s">
-        <v>44</v>
+        <v>4</v>
+      </c>
+      <c r="M14">
+        <v>28.35</v>
       </c>
       <c r="N14">
-        <v>6</v>
+        <v>4.33</v>
       </c>
       <c r="O14" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C15" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+      <c r="E15">
+        <v>92</v>
+      </c>
+      <c r="F15">
         <v>84</v>
       </c>
-      <c r="D15" t="s">
-        <v>85</v>
-      </c>
-      <c r="E15">
-        <v>15</v>
-      </c>
-      <c r="F15">
-        <v>10</v>
-      </c>
       <c r="G15">
-        <v>37</v>
+        <v>2060</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>10</v>
+        <v>104</v>
       </c>
       <c r="J15">
-        <v>7.4</v>
+        <v>29.01</v>
       </c>
       <c r="K15">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="L15">
-        <v>1</v>
-      </c>
-      <c r="M15">
-        <v>32.18</v>
+        <v>0</v>
+      </c>
+      <c r="M15" t="s">
+        <v>44</v>
       </c>
       <c r="N15">
-        <v>6.15</v>
+        <v>6</v>
       </c>
       <c r="O15" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>145</v>
       </c>
       <c r="B16" t="s">
-        <v>88</v>
+        <v>146</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>147</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>142</v>
       </c>
       <c r="E16">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>10</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16" t="s">
+        <v>148</v>
+      </c>
+      <c r="J16">
+        <v>10</v>
+      </c>
+      <c r="K16">
         <v>4</v>
       </c>
-      <c r="G16">
-        <v>31</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16" t="s">
-        <v>90</v>
-      </c>
-      <c r="J16">
-        <v>10.33</v>
-      </c>
-      <c r="K16">
-        <v>8</v>
-      </c>
       <c r="L16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16">
-        <v>56.75</v>
+        <v>7.5</v>
       </c>
       <c r="N16">
-        <v>6.05</v>
+        <v>3.33</v>
       </c>
       <c r="O16" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>149</v>
       </c>
       <c r="B17" t="s">
-        <v>93</v>
+        <v>150</v>
       </c>
       <c r="C17" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>142</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H17">
         <v>0</v>
       </c>
-      <c r="I17" t="s">
-        <v>95</v>
+      <c r="I17">
+        <v>9</v>
       </c>
       <c r="J17">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L17">
         <v>0</v>
       </c>
-      <c r="M17">
-        <v>22.17</v>
+      <c r="M17" t="s">
+        <v>44</v>
       </c>
       <c r="N17">
-        <v>6.14</v>
+        <v>7</v>
       </c>
       <c r="O17" t="s">
-        <v>96</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="B18" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C18" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="D18" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="E18">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="F18">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="G18">
-        <v>1295</v>
+        <v>37</v>
       </c>
       <c r="H18">
-        <v>5</v>
-      </c>
-      <c r="I18" t="s">
-        <v>100</v>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>10</v>
       </c>
       <c r="J18">
-        <v>35</v>
+        <v>7.4</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="L18">
-        <v>0</v>
-      </c>
-      <c r="M18" t="s">
-        <v>44</v>
-      </c>
-      <c r="N18" t="s">
-        <v>44</v>
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>32.18</v>
+      </c>
+      <c r="N18">
+        <v>6.15</v>
+      </c>
+      <c r="O18" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C19" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="D19" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E19">
-        <v>109</v>
+        <v>10</v>
       </c>
       <c r="F19">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="G19">
-        <v>3724</v>
+        <v>31</v>
       </c>
       <c r="H19">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I19" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="J19">
-        <v>36.869999999999997</v>
+        <v>10.33</v>
       </c>
       <c r="K19">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M19">
-        <v>35.47</v>
+        <v>57.22</v>
       </c>
       <c r="N19">
-        <v>5.88</v>
+        <v>6.06</v>
       </c>
       <c r="O19" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="C20" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="D20" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="E20">
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="F20">
-        <v>81</v>
+        <v>2</v>
       </c>
       <c r="G20">
-        <v>1316</v>
+        <v>12</v>
       </c>
       <c r="H20">
         <v>0</v>
       </c>
-      <c r="I20">
-        <v>60</v>
+      <c r="I20" t="s">
+        <v>95</v>
       </c>
       <c r="J20">
-        <v>19.64</v>
+        <v>6</v>
       </c>
       <c r="K20">
-        <v>183</v>
+        <v>6</v>
       </c>
       <c r="L20">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M20">
-        <v>20.48</v>
+        <v>22.17</v>
       </c>
       <c r="N20">
-        <v>4.24</v>
+        <v>6.14</v>
       </c>
       <c r="O20" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="C21" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="E21">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="F21">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="G21">
-        <v>120</v>
+        <v>1467</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I21" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="J21">
-        <v>30</v>
+        <v>37.619999999999997</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -1779,242 +1824,380 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E22">
-        <v>3</v>
+        <v>111</v>
       </c>
       <c r="F22">
-        <v>3</v>
+        <v>107</v>
       </c>
       <c r="G22">
-        <v>39</v>
+        <v>3730</v>
       </c>
       <c r="H22">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I22" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="J22">
-        <v>13</v>
+        <v>36.21</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L22">
-        <v>0</v>
-      </c>
-      <c r="M22" t="s">
-        <v>44</v>
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>35.47</v>
       </c>
       <c r="N22">
-        <v>5.33</v>
+        <v>5.88</v>
       </c>
       <c r="O22" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B23" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C23" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D23" t="s">
-        <v>28</v>
+        <v>109</v>
       </c>
       <c r="E23">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="F23">
-        <v>12</v>
+        <v>81</v>
       </c>
       <c r="G23">
-        <v>70</v>
+        <v>1316</v>
       </c>
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="I23" t="s">
-        <v>123</v>
+      <c r="I23">
+        <v>60</v>
       </c>
       <c r="J23">
-        <v>8.75</v>
+        <v>19.64</v>
       </c>
       <c r="K23">
-        <v>14</v>
+        <v>183</v>
       </c>
       <c r="L23">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M23">
-        <v>46.5</v>
+        <v>20.48</v>
       </c>
       <c r="N23">
-        <v>4.42</v>
+        <v>4.24</v>
       </c>
       <c r="O23" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C24" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E24">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="F24">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="G24">
-        <v>435</v>
+        <v>120</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="J24">
-        <v>25.59</v>
+        <v>30</v>
       </c>
       <c r="K24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24">
         <v>0</v>
       </c>
-      <c r="M24">
-        <v>34</v>
-      </c>
-      <c r="N24">
-        <v>5.37</v>
-      </c>
-      <c r="O24" t="s">
-        <v>129</v>
+      <c r="M24" t="s">
+        <v>44</v>
+      </c>
+      <c r="N24" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="B25" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="C25" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="D25" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="E25">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G25">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="H25">
         <v>0</v>
       </c>
       <c r="I25" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="J25">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="K25">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="L25">
         <v>0</v>
       </c>
-      <c r="M25">
-        <v>43.43</v>
+      <c r="M25" t="s">
+        <v>44</v>
       </c>
       <c r="N25">
-        <v>5.36</v>
+        <v>5.33</v>
       </c>
       <c r="O25" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="B26" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="C26" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E26">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="G26">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="J26">
-        <v>5</v>
+        <v>8.75</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
-      <c r="M26" t="s">
-        <v>44</v>
+      <c r="M26">
+        <v>46.5</v>
       </c>
       <c r="N26">
-        <v>6.29</v>
+        <v>4.42</v>
       </c>
       <c r="O26" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>139</v>
+        <v>125</v>
+      </c>
+      <c r="B27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27">
+        <v>17</v>
+      </c>
+      <c r="F27">
+        <v>17</v>
+      </c>
+      <c r="G27">
+        <v>435</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>128</v>
+      </c>
+      <c r="J27">
+        <v>25.59</v>
+      </c>
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>34</v>
+      </c>
+      <c r="N27">
+        <v>5.37</v>
+      </c>
+      <c r="O27" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" t="s">
+        <v>131</v>
+      </c>
+      <c r="C28" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" t="s">
+        <v>109</v>
+      </c>
+      <c r="E28">
+        <v>9</v>
+      </c>
+      <c r="F28">
+        <v>5</v>
+      </c>
+      <c r="G28">
+        <v>9</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28" t="s">
+        <v>133</v>
+      </c>
+      <c r="J28">
+        <v>3</v>
+      </c>
+      <c r="K28">
+        <v>7</v>
+      </c>
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>43.43</v>
+      </c>
+      <c r="N28">
+        <v>5.36</v>
+      </c>
+      <c r="O28" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>135</v>
+      </c>
+      <c r="B29" t="s">
+        <v>136</v>
+      </c>
+      <c r="C29" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>5</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+      <c r="I29" t="s">
+        <v>133</v>
+      </c>
+      <c r="J29">
+        <v>5</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29" t="s">
+        <v>44</v>
+      </c>
+      <c r="N29">
+        <v>6.29</v>
+      </c>
+      <c r="O29" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data Updation till 22 April 2024
</commit_message>
<xml_diff>
--- a/AFG_Player_Data.xlsx
+++ b/AFG_Player_Data.xlsx
@@ -824,7 +824,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="O32" sqref="O32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>